<commit_message>
finished and tested test suit w gcc, updated managament to include the change
</commit_message>
<xml_diff>
--- a/doc/test results.xlsx
+++ b/doc/test results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d78481ff72e5e73b/year 2/term2/lang_proc/langproc-2018-cw-OllieHarrietGroup/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{E362CB4F-0612-4286-B04B-83AC47571609}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{16B8293E-21D5-4A04-A4CD-BF7F75896FB5}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="8_{E362CB4F-0612-4286-B04B-83AC47571609}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{78E7EE51-3859-4A40-A833-D3C867FC7636}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{DD08D793-26D6-4E59-8FD9-2FC72D56836B}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
   <si>
     <t>type</t>
   </si>
@@ -64,6 +64,18 @@
   </si>
   <si>
     <t>op_gte_eq</t>
+  </si>
+  <si>
+    <t>function</t>
+  </si>
+  <si>
+    <t>func_invoke</t>
+  </si>
+  <si>
+    <t>IndentationError: expected an indented block</t>
+  </si>
+  <si>
+    <t>func_decl</t>
   </si>
 </sst>
 </file>
@@ -79,12 +91,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -99,8 +117,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8FF2EF8-23C6-4CC7-AAED-944F9987F958}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -440,69 +459,91 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>